<commit_message>
Add true ks and kd boundaries & Add more testing xlsx pairs
</commit_message>
<xml_diff>
--- a/data_kiwi/test.xlsx
+++ b/data_kiwi/test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="61">
   <si>
     <t xml:space="preserve">Protein</t>
   </si>
@@ -123,6 +123,30 @@
   </si>
   <si>
     <t xml:space="preserve">d2625.a1.a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acc01672.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d2543.a1.a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acc09753.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d1010.a1.a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acc09942.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d2512.a1.a1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acc11591.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">d3129.a1.a1</t>
   </si>
   <si>
     <t xml:space="preserve">Transcrit</t>
@@ -194,6 +218,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -279,365 +304,724 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AC8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C27" activeCellId="0" sqref="C27"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.54"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="0" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="0" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="0" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="0" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="0" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="0" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="0" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="0" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="0" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="0" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="0" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="0" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="0" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="0" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Z1" s="0" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AA1" s="0" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="0" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="0" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="1" t="n">
         <v>3.20228150815327</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>1.15916520235749</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="1" t="n">
         <v>1.18435422928546</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="1" t="n">
         <v>1.15082216029154</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>0.325011049676069</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="1" t="n">
         <v>0.415474072735003</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="1" t="n">
         <v>0.41361951439784</v>
       </c>
-      <c r="J2" s="0" t="n">
+      <c r="J2" s="1" t="n">
         <v>0.179696149329344</v>
       </c>
-      <c r="K2" s="0" t="n">
+      <c r="K2" s="1" t="n">
         <v>0.518327421749059</v>
       </c>
-      <c r="L2" s="0" t="n">
+      <c r="L2" s="1" t="n">
         <v>0.156350330396767</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>0.0923307703550274</v>
       </c>
-      <c r="N2" s="0" t="n">
+      <c r="N2" s="1" t="n">
         <v>0.225638243421686</v>
       </c>
-      <c r="O2" s="0" t="n">
+      <c r="O2" s="1" t="n">
         <v>0.129160983680973</v>
       </c>
-      <c r="P2" s="0" t="n">
+      <c r="P2" s="1" t="n">
         <v>0.0191898675512778</v>
       </c>
-      <c r="Q2" s="0" t="n">
+      <c r="Q2" s="1" t="n">
         <v>0.0256400567806329</v>
       </c>
-      <c r="R2" s="0" t="n">
+      <c r="R2" s="1" t="n">
         <v>0.0583075772851665</v>
       </c>
-      <c r="S2" s="0" t="n">
+      <c r="S2" s="1" t="n">
         <v>0.0243751723261681</v>
       </c>
-      <c r="T2" s="0" t="n">
+      <c r="T2" s="1" t="n">
         <v>0.0213820246693683</v>
       </c>
-      <c r="U2" s="0" t="n">
+      <c r="U2" s="1" t="n">
         <v>0.0587182661659283</v>
       </c>
-      <c r="V2" s="0" t="n">
+      <c r="V2" s="1" t="n">
         <v>0.0230435800041032</v>
       </c>
-      <c r="W2" s="0" t="n">
+      <c r="W2" s="1" t="n">
         <v>0.0262613787825933</v>
       </c>
-      <c r="X2" s="0" t="n">
+      <c r="X2" s="1" t="n">
         <v>0.0571568134003593</v>
       </c>
-      <c r="Y2" s="0" t="n">
+      <c r="Y2" s="1" t="n">
         <v>0.0197004776346475</v>
       </c>
-      <c r="Z2" s="0" t="n">
+      <c r="Z2" s="1" t="n">
         <v>0.0227362892496546</v>
       </c>
-      <c r="AA2" s="0" t="n">
+      <c r="AA2" s="1" t="n">
         <v>0.031563735120124</v>
       </c>
-      <c r="AB2" s="0" t="n">
+      <c r="AB2" s="1" t="n">
         <v>0.00601641129637127</v>
       </c>
-      <c r="AC2" s="0" t="n">
+      <c r="AC2" s="1" t="n">
         <v>0.00627186863612194</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>3.15812230344946</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>1.36503384715201</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>1.26473263616481</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>1.5909667079626</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>0.504228686330727</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>0.566174422468401</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>0.748900271892983</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <v>0.276937886702825</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>0.773141875148984</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="1" t="n">
         <v>0.311714897902889</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>0.178801115486559</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>0.409142959890641</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <v>0.190921828427845</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="P3" s="1" t="n">
         <v>0.0285880869385937</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <v>0.0378524271301584</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>0.0795621620499178</v>
       </c>
-      <c r="S3" s="0" t="n">
+      <c r="S3" s="1" t="n">
         <v>0.0324948851275826</v>
       </c>
-      <c r="T3" s="0" t="n">
+      <c r="T3" s="1" t="n">
         <v>0.0302818147072873</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3" s="1" t="n">
         <v>0.0625900820250001</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3" s="1" t="n">
         <v>0.0192955721529138</v>
       </c>
-      <c r="W3" s="0" t="n">
+      <c r="W3" s="1" t="n">
         <v>0.0246170610350049</v>
       </c>
-      <c r="X3" s="0" t="n">
+      <c r="X3" s="1" t="n">
         <v>0.0687542297265726</v>
       </c>
-      <c r="Y3" s="0" t="n">
+      <c r="Y3" s="1" t="n">
         <v>0.0217412959745226</v>
       </c>
-      <c r="Z3" s="0" t="n">
+      <c r="Z3" s="1" t="n">
         <v>0.023936897582389</v>
       </c>
-      <c r="AA3" s="0" t="n">
+      <c r="AA3" s="1" t="n">
         <v>0.0697511378856484</v>
       </c>
-      <c r="AB3" s="0" t="n">
+      <c r="AB3" s="1" t="n">
         <v>0.0136518215962496</v>
       </c>
-      <c r="AC3" s="0" t="n">
+      <c r="AC3" s="1" t="n">
         <v>0.0141757360341989</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>0.418990562131434</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>0.153659712948818</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="1" t="n">
         <v>0.147834777073171</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="1" t="n">
         <v>0.30180220560164</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="1" t="n">
         <v>0.0846573298134432</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="1" t="n">
         <v>0.0894077921661187</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="1" t="n">
         <v>0.0879573673458679</v>
       </c>
-      <c r="J4" s="0" t="n">
+      <c r="J4" s="1" t="n">
         <v>0.045278374471397</v>
       </c>
-      <c r="K4" s="0" t="n">
+      <c r="K4" s="1" t="n">
         <v>0.110912983319787</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L4" s="1" t="n">
         <v>0.0440914511871455</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="1" t="n">
         <v>0.0223092221663425</v>
       </c>
-      <c r="N4" s="0" t="n">
+      <c r="N4" s="1" t="n">
         <v>0.043000256945688</v>
       </c>
-      <c r="O4" s="0" t="n">
+      <c r="O4" s="1" t="n">
         <v>0.0194518133101595</v>
       </c>
-      <c r="P4" s="0" t="n">
+      <c r="P4" s="1" t="n">
         <v>0.00324788269688288</v>
       </c>
-      <c r="Q4" s="0" t="n">
+      <c r="Q4" s="1" t="n">
         <v>0.00424756874637721</v>
       </c>
-      <c r="R4" s="0" t="n">
+      <c r="R4" s="1" t="n">
         <v>0.011075374653384</v>
       </c>
-      <c r="S4" s="0" t="n">
+      <c r="S4" s="1" t="n">
         <v>0.00452846415045328</v>
       </c>
-      <c r="T4" s="0" t="n">
+      <c r="T4" s="1" t="n">
         <v>0.00401476992908872</v>
       </c>
-      <c r="U4" s="0" t="n">
+      <c r="U4" s="1" t="n">
         <v>0.00964894128521989</v>
       </c>
-      <c r="V4" s="0" t="n">
+      <c r="V4" s="1" t="n">
         <v>0.0031182166846939</v>
       </c>
-      <c r="W4" s="0" t="n">
+      <c r="W4" s="1" t="n">
         <v>0.0038909377542269</v>
       </c>
-      <c r="X4" s="0" t="n">
+      <c r="X4" s="1" t="n">
         <v>0.0115500078102036</v>
       </c>
-      <c r="Y4" s="0" t="n">
+      <c r="Y4" s="1" t="n">
         <v>0.00404107180552816</v>
       </c>
-      <c r="Z4" s="0" t="n">
+      <c r="Z4" s="1" t="n">
         <v>0.00492828490815292</v>
       </c>
-      <c r="AA4" s="0" t="n">
+      <c r="AA4" s="1" t="n">
         <v>0.0192755639585246</v>
       </c>
-      <c r="AB4" s="0" t="n">
+      <c r="AB4" s="1" t="n">
         <v>0.00323519085362168</v>
       </c>
-      <c r="AC4" s="0" t="n">
+      <c r="AC4" s="1" t="n">
         <v>0.00404289132682335</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>1.89524412699994</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.847545282149878</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.840276388377382</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.955166017351793</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>0.281745755386297</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.349581337241442</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>0.356907707801369</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>0.169681902640592</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.431867386537049</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0.154484801198911</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0.0975838912995475</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>0.216389456827878</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>0.127920625489446</v>
+      </c>
+      <c r="P5" s="0" t="n">
+        <v>0.0214649648257197</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <v>0.0257979238540665</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <v>0.0437462052700071</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <v>0.0183829246816933</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <v>0.0177494952343411</v>
+      </c>
+      <c r="U5" s="0" t="n">
+        <v>0.0363698667678341</v>
+      </c>
+      <c r="V5" s="0" t="n">
+        <v>0.0142229599575434</v>
+      </c>
+      <c r="W5" s="0" t="n">
+        <v>0.0160183901124699</v>
+      </c>
+      <c r="X5" s="0" t="n">
+        <v>0.0458220543229604</v>
+      </c>
+      <c r="Y5" s="0" t="n">
+        <v>0.0175066103716484</v>
+      </c>
+      <c r="Z5" s="0" t="n">
+        <v>0.0198433253096299</v>
+      </c>
+      <c r="AA5" s="0" t="n">
+        <v>0.0478306505495341</v>
+      </c>
+      <c r="AB5" s="0" t="n">
+        <v>0.00928734515230559</v>
+      </c>
+      <c r="AC5" s="0" t="n">
+        <v>0.0102428997847506</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>90.9493676320012</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>34.0525984987877</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>29.1896412686499</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>120.618223926652</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>36.0578907804566</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>47.0108045171392</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>54.9003809546367</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>22.5770663858682</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>65.0266182222619</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>25.6566684762643</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>15.4887068242438</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>37.3287636996131</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>18.2149958635798</v>
+      </c>
+      <c r="P6" s="0" t="n">
+        <v>3.21855980188916</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <v>3.6739938752881</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <v>2.21476239308126</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <v>0.861879597787647</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <v>0.815151619576383</v>
+      </c>
+      <c r="U6" s="0" t="n">
+        <v>0.628103012982436</v>
+      </c>
+      <c r="V6" s="0" t="n">
+        <v>0.195438074686644</v>
+      </c>
+      <c r="W6" s="0" t="n">
+        <v>0.234350564336726</v>
+      </c>
+      <c r="X6" s="0" t="n">
+        <v>0.4228131409949</v>
+      </c>
+      <c r="Y6" s="0" t="n">
+        <v>0.159971521305012</v>
+      </c>
+      <c r="Z6" s="0" t="n">
+        <v>0.17934505007769</v>
+      </c>
+      <c r="AA6" s="0" t="n">
+        <v>0.756343660655848</v>
+      </c>
+      <c r="AB6" s="0" t="n">
+        <v>0.15785006268173</v>
+      </c>
+      <c r="AC6" s="0" t="n">
+        <v>0.17128774039321</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>4.4477304074931</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1.77714617254608</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1.77851487653532</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1.9420661263591</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>0.529291412353143</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>0.683312041944036</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>0.520171397699618</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>0.222630594552315</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0.650058247122261</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0.18081205875144</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>0.106873825816056</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>0.268490088362992</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>0.153538075488508</v>
+      </c>
+      <c r="P7" s="0" t="n">
+        <v>0.0196593012571685</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <v>0.0248238704853235</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <v>0.0478881549991955</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <v>0.0199567451781263</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <v>0.0185926972362988</v>
+      </c>
+      <c r="U7" s="0" t="n">
+        <v>0.0297469635535014</v>
+      </c>
+      <c r="V7" s="0" t="n">
+        <v>0.0119293504864271</v>
+      </c>
+      <c r="W7" s="0" t="n">
+        <v>0.0141963330491146</v>
+      </c>
+      <c r="X7" s="0" t="n">
+        <v>0.0329436483796461</v>
+      </c>
+      <c r="Y7" s="0" t="n">
+        <v>0.0108415831340259</v>
+      </c>
+      <c r="Z7" s="0" t="n">
+        <v>0.0120478251608761</v>
+      </c>
+      <c r="AA7" s="0" t="n">
+        <v>0.0382312893419584</v>
+      </c>
+      <c r="AB7" s="0" t="n">
+        <v>0.00880592068213322</v>
+      </c>
+      <c r="AC7" s="0" t="n">
+        <v>0.0105348579351496</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>2.32330227053817</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>1.1490373622993</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>1.11209575604404</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>1.96882487098446</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0.496820855754138</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <v>0.639126315713339</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>0.69513953961967</v>
+      </c>
+      <c r="J8" s="0" t="n">
+        <v>0.301738699666247</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.9470135120876</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>0.261578663427966</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>0.158480708905398</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>0.36149440531948</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>0.236618489036893</v>
+      </c>
+      <c r="P8" s="0" t="n">
+        <v>0.0544194845421009</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <v>0.0562751684722985</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <v>0.143776681630596</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <v>0.0615339587403497</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <v>0.0623344110339065</v>
+      </c>
+      <c r="U8" s="0" t="n">
+        <v>0.142563473260967</v>
+      </c>
+      <c r="V8" s="0" t="n">
+        <v>0.0554133688940992</v>
+      </c>
+      <c r="W8" s="0" t="n">
+        <v>0.0644730259731622</v>
+      </c>
+      <c r="X8" s="0" t="n">
+        <v>0.121565043632364</v>
+      </c>
+      <c r="Y8" s="0" t="n">
+        <v>0.0448686021239713</v>
+      </c>
+      <c r="Z8" s="0" t="n">
+        <v>0.0534961573426924</v>
+      </c>
+      <c r="AA8" s="0" t="n">
+        <v>0.171761356419071</v>
+      </c>
+      <c r="AB8" s="0" t="n">
+        <v>0.0299866661168692</v>
+      </c>
+      <c r="AC8" s="0" t="n">
+        <v>0.0328335325587041</v>
       </c>
     </row>
   </sheetData>
@@ -656,98 +1040,101 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AC4"/>
+  <dimension ref="A1:AC8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.54"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="0" t="n">
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="D1" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="F1" s="0" t="n">
+      <c r="D1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F1" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="G1" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="H1" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="I1" s="0" t="n">
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="1" t="n">
         <v>39</v>
       </c>
-      <c r="K1" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="0" t="n">
-        <v>39</v>
-      </c>
-      <c r="M1" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="O1" s="0" t="n">
+      <c r="M1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="O1" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="P1" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q1" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="R1" s="0" t="n">
+      <c r="P1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="1" t="n">
         <v>76</v>
       </c>
-      <c r="S1" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="T1" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" s="0" t="n">
+      <c r="S1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="U1" s="1" t="n">
         <v>118</v>
       </c>
-      <c r="V1" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="W1" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="X1" s="0" t="n">
+      <c r="V1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="X1" s="1" t="n">
         <v>179</v>
       </c>
-      <c r="Y1" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z1" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="AA1" s="0" t="n">
+      <c r="Y1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA1" s="1" t="n">
         <v>222</v>
       </c>
-      <c r="AB1" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC1" s="0" t="s">
-        <v>52</v>
+      <c r="AB1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -840,91 +1227,91 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="1" t="n">
         <v>57595.0702531612</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>168002.336866387</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="1" t="n">
         <v>190705.288809914</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="1" t="n">
         <v>123946.13810815</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="1" t="n">
         <v>107149.185515952</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="1" t="n">
         <v>70914.5993254812</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="1" t="n">
         <v>41529.0195883954</v>
       </c>
-      <c r="J3" s="0" t="n">
+      <c r="J3" s="1" t="n">
         <v>31604.6981330588</v>
       </c>
-      <c r="K3" s="0" t="n">
+      <c r="K3" s="1" t="n">
         <v>24563.5300541578</v>
       </c>
-      <c r="L3" s="0" t="n">
+      <c r="L3" s="1" t="n">
         <v>30391.9706389273</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>27269.5230889483</v>
       </c>
-      <c r="N3" s="0" t="n">
+      <c r="N3" s="1" t="n">
         <v>9150.94267149111</v>
       </c>
-      <c r="O3" s="0" t="n">
+      <c r="O3" s="1" t="n">
         <v>28906.1252021889</v>
       </c>
-      <c r="P3" s="0" t="n">
+      <c r="P3" s="1" t="n">
         <v>34820.9846532158</v>
       </c>
-      <c r="Q3" s="0" t="n">
+      <c r="Q3" s="1" t="n">
         <v>36726.7404481005</v>
       </c>
-      <c r="R3" s="0" t="n">
+      <c r="R3" s="1" t="n">
         <v>58432.2677618415</v>
       </c>
-      <c r="S3" s="0" t="n">
+      <c r="S3" s="1" t="n">
         <v>62504.7725419246</v>
       </c>
-      <c r="T3" s="0" t="n">
+      <c r="T3" s="1" t="n">
         <v>25066.086888526</v>
       </c>
-      <c r="U3" s="0" t="n">
+      <c r="U3" s="1" t="n">
         <v>29794.620190065</v>
       </c>
-      <c r="V3" s="0" t="n">
+      <c r="V3" s="1" t="n">
         <v>10578.9278304721</v>
       </c>
-      <c r="W3" s="0" t="n">
+      <c r="W3" s="1" t="n">
         <v>14461.513040357</v>
       </c>
-      <c r="X3" s="0" t="n">
+      <c r="X3" s="1" t="n">
         <v>19144.5902889265</v>
       </c>
-      <c r="Y3" s="0" t="n">
+      <c r="Y3" s="1" t="n">
         <v>98859.7784516968</v>
       </c>
-      <c r="Z3" s="0" t="n">
+      <c r="Z3" s="1" t="n">
         <v>39716.4849130383</v>
       </c>
-      <c r="AA3" s="0" t="n">
+      <c r="AA3" s="1" t="n">
         <v>28371.2073630246</v>
       </c>
-      <c r="AB3" s="0" t="n">
+      <c r="AB3" s="1" t="n">
         <v>17479.1342546269</v>
       </c>
-      <c r="AC3" s="0" t="n">
+      <c r="AC3" s="1" t="n">
         <v>23880.1298607118</v>
       </c>
     </row>
@@ -1017,10 +1404,366 @@
         <v>1931.30069721228</v>
       </c>
     </row>
+    <row r="5" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>54906.6670662961</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>45378.4431689608</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>45095.9851985272</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>46060.6436645047</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>48792.2247738362</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>45530.6991305168</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>10861.4681897264</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <v>15435.5223740772</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <v>15288.0200145937</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <v>7573.17492051737</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <v>6778.55878287527</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <v>4576.3955175836</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <v>5133.81649301576</v>
+      </c>
+      <c r="P5" s="1" t="n">
+        <v>4168.38648166075</v>
+      </c>
+      <c r="Q5" s="1" t="n">
+        <v>8460.29705450206</v>
+      </c>
+      <c r="R5" s="1" t="n">
+        <v>1776.07492557605</v>
+      </c>
+      <c r="S5" s="1" t="n">
+        <v>1235.62425553805</v>
+      </c>
+      <c r="T5" s="1" t="n">
+        <v>1716.66811874578</v>
+      </c>
+      <c r="U5" s="1" t="n">
+        <v>2162.65943367502</v>
+      </c>
+      <c r="V5" s="1" t="n">
+        <v>3127.19077218863</v>
+      </c>
+      <c r="W5" s="1" t="n">
+        <v>2454.24031402716</v>
+      </c>
+      <c r="X5" s="1" t="n">
+        <v>3411.6398663577</v>
+      </c>
+      <c r="Y5" s="1" t="n">
+        <v>2782.33216471673</v>
+      </c>
+      <c r="Z5" s="1" t="n">
+        <v>5355.95072484091</v>
+      </c>
+      <c r="AA5" s="1" t="n">
+        <v>1628.81386114591</v>
+      </c>
+      <c r="AB5" s="1" t="n">
+        <v>1762.03774127131</v>
+      </c>
+      <c r="AC5" s="1" t="n">
+        <v>3069.48249471463</v>
+      </c>
+    </row>
+    <row r="6" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>75283.9560821077</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>62594.432027661</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>64681.2799725916</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>132285.45782369</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>130611.754224026</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>127812.54885821</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>43154.7943866983</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <v>58098.7076328568</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <v>59935.3734065645</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <v>26224.5027273823</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <v>21990.0145697898</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <v>15965.5829990499</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <v>17249.1528203947</v>
+      </c>
+      <c r="P6" s="1" t="n">
+        <v>13656.9242734861</v>
+      </c>
+      <c r="Q6" s="1" t="n">
+        <v>28941.9709929667</v>
+      </c>
+      <c r="R6" s="1" t="n">
+        <v>5195.91204443654</v>
+      </c>
+      <c r="S6" s="1" t="n">
+        <v>3150.09748359311</v>
+      </c>
+      <c r="T6" s="1" t="n">
+        <v>4205.19441386885</v>
+      </c>
+      <c r="U6" s="1" t="n">
+        <v>5094.36496237017</v>
+      </c>
+      <c r="V6" s="1" t="n">
+        <v>6026.61800418987</v>
+      </c>
+      <c r="W6" s="1" t="n">
+        <v>5635.28243410162</v>
+      </c>
+      <c r="X6" s="1" t="n">
+        <v>3214.14541102799</v>
+      </c>
+      <c r="Y6" s="1" t="n">
+        <v>2408.06406915963</v>
+      </c>
+      <c r="Z6" s="1" t="n">
+        <v>5443.84560208279</v>
+      </c>
+      <c r="AA6" s="1" t="n">
+        <v>2609.34194729191</v>
+      </c>
+      <c r="AB6" s="1" t="n">
+        <v>2729.25818134479</v>
+      </c>
+      <c r="AC6" s="1" t="n">
+        <v>3924.64186290511</v>
+      </c>
+    </row>
+    <row r="7" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>25563.882306064</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>27235.8668901147</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>30727.8369241373</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>64053.1293471856</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>66218.7234993218</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>71461.2062016693</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>15379.2692538894</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <v>20549.9756447027</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <v>23186.2844965673</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <v>10994.845250934</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <v>9435.20575994421</v>
+      </c>
+      <c r="N7" s="1" t="n">
+        <v>7090.45638816941</v>
+      </c>
+      <c r="O7" s="1" t="n">
+        <v>5230.4801096712</v>
+      </c>
+      <c r="P7" s="1" t="n">
+        <v>4329.33203185193</v>
+      </c>
+      <c r="Q7" s="1" t="n">
+        <v>9560.30034204394</v>
+      </c>
+      <c r="R7" s="1" t="n">
+        <v>4655.42094169259</v>
+      </c>
+      <c r="S7" s="1" t="n">
+        <v>1285.44951877267</v>
+      </c>
+      <c r="T7" s="1" t="n">
+        <v>1902.87909772858</v>
+      </c>
+      <c r="U7" s="1" t="n">
+        <v>2562.60247038439</v>
+      </c>
+      <c r="V7" s="1" t="n">
+        <v>3033.72920676233</v>
+      </c>
+      <c r="W7" s="1" t="n">
+        <v>1760.77341450673</v>
+      </c>
+      <c r="X7" s="1" t="n">
+        <v>2300.54964497065</v>
+      </c>
+      <c r="Y7" s="1" t="n">
+        <v>2039.62408006525</v>
+      </c>
+      <c r="Z7" s="1" t="n">
+        <v>4468.65598990881</v>
+      </c>
+      <c r="AA7" s="1" t="n">
+        <v>1309.00971005918</v>
+      </c>
+      <c r="AB7" s="1" t="n">
+        <v>1103.40549227051</v>
+      </c>
+      <c r="AC7" s="1" t="n">
+        <v>2127.05949237761</v>
+      </c>
+    </row>
+    <row r="8" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>62174.1693058733</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>54056.4537947078</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>57064.6220532441</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>60186.9944882749</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>69675.2962509367</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>64628.3284137834</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>12862.2843543605</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <v>16855.2862677706</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <v>17874.1974328916</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <v>9280.10873785885</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <v>7901.66329177675</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <v>5389.67763798611</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <v>5375.80249567116</v>
+      </c>
+      <c r="P8" s="1" t="n">
+        <v>4256.93364676428</v>
+      </c>
+      <c r="Q8" s="1" t="n">
+        <v>9063.88439950168</v>
+      </c>
+      <c r="R8" s="1" t="n">
+        <v>3806.52874724912</v>
+      </c>
+      <c r="S8" s="1" t="n">
+        <v>2163.3763234534</v>
+      </c>
+      <c r="T8" s="1" t="n">
+        <v>2889.18140338464</v>
+      </c>
+      <c r="U8" s="1" t="n">
+        <v>4455.62805116222</v>
+      </c>
+      <c r="V8" s="1" t="n">
+        <v>4768.32202766528</v>
+      </c>
+      <c r="W8" s="1" t="n">
+        <v>3789.54796531716</v>
+      </c>
+      <c r="X8" s="1" t="n">
+        <v>8467.49517032084</v>
+      </c>
+      <c r="Y8" s="1" t="n">
+        <v>7240.40805760115</v>
+      </c>
+      <c r="Z8" s="1" t="n">
+        <v>15175.3201830164</v>
+      </c>
+      <c r="AA8" s="1" t="n">
+        <v>4877.06743865487</v>
+      </c>
+      <c r="AB8" s="1" t="n">
+        <v>5003.93574425127</v>
+      </c>
+      <c r="AC8" s="1" t="n">
+        <v>7566.0849661496</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Erregularra"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Erregularra"&amp;12Orrialdea &amp;P</oddFooter>

</xml_diff>